<commit_message>
Add constant memory use for rowPointers and destka
</commit_message>
<xml_diff>
--- a/BFS_time.xlsx
+++ b/BFS_time.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://polimi365-my.sharepoint.com/personal/10799547_polimi_it/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matte\CLionProjects\BFS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4425A67B-9419-427E-A907-FD0E99FFD274}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DA46E77-E675-454B-8CBB-D5C6418C4908}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{EFEA939A-6BC7-452C-A878-25D35D9D7F79}"/>
   </bookViews>
@@ -36,12 +36,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>CPU VERSION</t>
   </si>
   <si>
     <t>GPU V1</t>
+  </si>
+  <si>
+    <t>GPU V2</t>
+  </si>
+  <si>
+    <t>add constant memory for rowPointers and destinations</t>
+  </si>
+  <si>
+    <t>GPU v3</t>
   </si>
 </sst>
 </file>
@@ -49,7 +58,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="#,##0.000000"/>
+    <numFmt numFmtId="164" formatCode="#,##0.000000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -81,7 +90,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -416,64 +425,91 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAEEB0AD-91A6-440C-A732-793A1DA8936E}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="11.3984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.1328125" customWidth="1"/>
+    <col min="3" max="3" width="9.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>3.4000000000000002E-2</v>
       </c>
       <c r="B2" s="1">
         <v>87.016998000000001</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C2">
+        <v>24.364999999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>3.2000000000000001E-2</v>
       </c>
       <c r="B3" s="1">
         <v>85.563004000000006</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C3">
+        <v>20.271000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>3.3000000000000002E-2</v>
       </c>
       <c r="B4" s="1">
         <v>85.129997000000003</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C4">
+        <v>15.59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>4.8000000000000001E-2</v>
       </c>
       <c r="B5" s="1">
         <v>85.516998000000001</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C5" s="1">
+        <v>19.966999000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>3.3000000000000002E-2</v>
       </c>
       <c r="B6" s="1">
         <v>85.401000999999994</v>
+      </c>
+      <c r="C6">
+        <v>15.97</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C7" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>